<commit_message>
at least fix single client
</commit_message>
<xml_diff>
--- a/blacklist/subcodes_C.xlsx
+++ b/blacklist/subcodes_C.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="69" documentId="8_{BE348F34-2D8B-4C2A-83EE-F3D110E92086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{059052D5-300F-114C-98A1-3267540F7FE7}"/>
   <bookViews>
-    <workbookView xWindow="10620" yWindow="3200" windowWidth="29400" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13660" yWindow="4220" windowWidth="29400" windowHeight="16740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1 - subcodes_C" sheetId="1" r:id="rId1"/>
@@ -1641,11 +1641,11 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1730,6 +1730,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2780,7 +2784,7 @@
   <dimension ref="A1:E211"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1"/>
@@ -2794,12 +2798,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="27.5" customHeight="1">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
     </row>
     <row r="2" spans="1:5" ht="20.25" customHeight="1">
       <c r="A2" s="2" t="s">
@@ -2814,7 +2818,7 @@
       <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="13" t="s">
         <v>465</v>
       </c>
     </row>

</xml_diff>